<commit_message>
Correção de DSS e diagrama packages feito
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/EscolherConfiguracaoOtima.xlsx
+++ b/Modelos UML/Descrição UseCases/EscolherConfiguracaoOtima.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eu\Desktop\UM\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Actor input</t>
   </si>
@@ -81,49 +81,58 @@
     <t>2.Mostra opções</t>
   </si>
   <si>
-    <t>8. Mostra melhor carro e suas especificações</t>
-  </si>
-  <si>
-    <t>10. Regista e verifica alterações</t>
-  </si>
-  <si>
-    <t>11. Pergunta se pretende confirmar</t>
-  </si>
-  <si>
-    <t>12. Confirma compra</t>
-  </si>
-  <si>
     <t>13. Confirma compra</t>
   </si>
   <si>
-    <t>14. Insere carro na fila para produção</t>
-  </si>
-  <si>
     <t>Regressa a 9</t>
   </si>
   <si>
-    <t>12.1 Não confirma compra</t>
-  </si>
-  <si>
-    <t>Alternativo 2 [Não confirma compra] (passo 12)</t>
-  </si>
-  <si>
-    <t>Alternativo 1 [Componentes incompativeis] (passo 10)</t>
-  </si>
-  <si>
-    <t>10.1 Verifica que escolheu peças incompatíveis</t>
-  </si>
-  <si>
-    <t>10.2 Mostra peças incompatíveis e/ou peças em falta</t>
-  </si>
-  <si>
-    <t>9.Escolhe especificações adicionais e altera (ou não) especificações ótimas</t>
+    <t>8. Calcula preço</t>
+  </si>
+  <si>
+    <t>9. Mostra melhor carro, preço e suas especificações</t>
+  </si>
+  <si>
+    <t>10.Escolhe especificações adicionais e altera (ou não) especificações ótimas</t>
+  </si>
+  <si>
+    <t>11. Regista e verifica alterações</t>
+  </si>
+  <si>
+    <t>12. Pergunta se pretende confirmar</t>
+  </si>
+  <si>
+    <t>14. Confirma compra</t>
+  </si>
+  <si>
+    <t>15. Insere carro na fila para produção</t>
+  </si>
+  <si>
+    <t>Alternativo 1 [Componentes incompativeis] (passo 11)</t>
+  </si>
+  <si>
+    <t>Alternativo 2 [Não confirma compra] (passo 13)</t>
+  </si>
+  <si>
+    <t>13.1 Não confirma compra</t>
+  </si>
+  <si>
+    <t>11.1 Mostra peças incompatíveis e/ou peças em falta</t>
+  </si>
+  <si>
+    <t>Alternativo 3 [Muda peças] (passo 10)</t>
+  </si>
+  <si>
+    <t>Regressa a 11</t>
+  </si>
+  <si>
+    <t>10.1 Verifica que a configuração ótima foi alterada e recalcula preço</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -154,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -239,6 +248,73 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -249,7 +325,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -260,7 +336,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -274,64 +350,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -340,9 +358,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -353,54 +369,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,228 +740,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D28"/>
+  <dimension ref="B1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.625" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="4" width="71.625" customWidth="1"/>
+    <col min="3" max="3" width="72.875" customWidth="1"/>
+    <col min="4" max="4" width="71.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="23"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="23"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="23"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="23"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="23"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="22"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="22"/>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="22"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="22"/>
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="23"/>
-      <c r="C15" s="5" t="s">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="22"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="23"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
+    </row>
+    <row r="23" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="16"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="23"/>
-      <c r="C18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="23"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="23"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="2" t="s">
+    <row r="24" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="16"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="16"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="17"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="1" t="s">
+      <c r="C27" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="17"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="17"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="2:4" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" s="11" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="3"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="14"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" s="10" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="24"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="25"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B21:B24"/>
+  <mergeCells count="8">
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B22:B26"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B20"/>
+    <mergeCell ref="B6:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterei alt para opt e para break
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/EscolherConfiguracaoOtima.xlsx
+++ b/Modelos UML/Descrição UseCases/EscolherConfiguracaoOtima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959CEA43-01CC-4C97-97D6-C83F462B5F40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69453B79-2208-401C-9B2E-EF04F340136E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Actor input</t>
   </si>
@@ -100,13 +100,10 @@
     <t>13. Insere carro na fila para produção</t>
   </si>
   <si>
-    <t>Alternativo 2 [Não confirma compra] (passo 11)</t>
-  </si>
-  <si>
     <t>11.1 Não confirma compra</t>
   </si>
   <si>
-    <t>Regressa a 1</t>
+    <t>Exceção 1 [Não confirma compra] (passo 11)</t>
   </si>
 </sst>
 </file>
@@ -675,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -828,19 +825,17 @@
     </row>
     <row r="20" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="14"/>

</xml_diff>